<commit_message>
Implemented Pdf Data Extraction Code
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/SummaryReport.xlsx
+++ b/BE_LTD_Dispatcher/Data/SummaryReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_922A42F19279F722C60B368C938291CA7F1A5F4A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63FF4A22-7824-48B4-A58D-99030336B81E}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_A3CA21ED92A976BF6D96A6853905B85C7E1A4443" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A3B5BBB-A053-4C86-AD68-4F4384EF7A47}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Subject</t>
   </si>
@@ -37,6 +37,18 @@
     <t>Attachment Unprotected Status</t>
   </si>
   <si>
+    <t>Employee Number</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>CIN Number</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Statement SBI Bank</t>
   </si>
   <si>
@@ -50,6 +62,18 @@
   </si>
   <si>
     <t>Password Removed</t>
+  </si>
+  <si>
+    <t>1182</t>
+  </si>
+  <si>
+    <t>280701501966,</t>
+  </si>
+  <si>
+    <t>U72200TG2014PTC092878</t>
+  </si>
+  <si>
+    <t>May-2022</t>
   </si>
   <si>
     <t>Attachment Not Found</t>
@@ -409,9 +433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -420,9 +446,12 @@
     <col min="3" max="3" width="117.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,81 +467,141 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
+      <c r="I6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Each Bank Subject In Config File
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/SummaryReport.xlsx
+++ b/BE_LTD_Dispatcher/Data/SummaryReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_A3CA21ED9289F505046BE4DE612982C95B024417" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8644DB16-DE85-4D67-AA48-655F579C2B0A}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_BFC262E792397E787547C3E9E5879E387F1A84B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F45F496-D8B7-45EE-9928-4F1FBBCE1DE7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,13 +49,16 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Statement SBI Bank</t>
+    <t>SBI Statement</t>
+  </si>
+  <si>
+    <t>Attachment Not Found</t>
   </si>
   <si>
     <t>Attachment Found</t>
   </si>
   <si>
-    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-23-2022\SBI Bank\Vidya Sagar Reddy.pdf</t>
+    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-24-2022\SBI Bank\Vidya Sagar Reddy.pdf</t>
   </si>
   <si>
     <t>Password Found</t>
@@ -76,25 +79,22 @@
     <t>May-2022</t>
   </si>
   <si>
-    <t>Attachment Not Found</t>
-  </si>
-  <si>
-    <t>Statement Axis Bank</t>
-  </si>
-  <si>
-    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-23-2022\Axis Bank\Vidya Sagar Reddy.pdf</t>
-  </si>
-  <si>
-    <t>Statement ICICI Bank</t>
-  </si>
-  <si>
-    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-23-2022\ICICI Bank\Vidya Sagar Reddy.pdf</t>
-  </si>
-  <si>
-    <t>Statement HDFC Bank</t>
-  </si>
-  <si>
-    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-23-2022\HDFC Bank\Vidya Sagar Reddy.pdf</t>
+    <t>AXIS Statement</t>
+  </si>
+  <si>
+    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-24-2022\Axis Bank\Vidya Sagar Reddy.pdf</t>
+  </si>
+  <si>
+    <t>ICICI Statement</t>
+  </si>
+  <si>
+    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-24-2022\ICICI Bank\Vidya Sagar Reddy.pdf</t>
+  </si>
+  <si>
+    <t>HDFC Statement</t>
+  </si>
+  <si>
+    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\06-24-2022\HDFC Bank\Vidya Sagar Reddy.pdf</t>
   </si>
 </sst>
 </file>
@@ -435,13 +435,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="128" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
@@ -449,7 +447,6 @@
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -488,33 +485,33 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -523,28 +520,28 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -552,28 +549,28 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -581,28 +578,28 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>